<commit_message>
Convert to one time through mode.  Needs some refactoring.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="380">
   <si>
     <t>Property</t>
   </si>
@@ -1154,6 +1154,9 @@
   </si>
   <si>
     <t>General diagnostic testing</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1516,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1586,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,7 +2578,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -2586,7 +2589,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Added year two bugs to SNOMED mapping in Config.xlsx
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="390">
   <si>
     <t>Property</t>
   </si>
@@ -1157,6 +1157,36 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>Pasteurella multocida</t>
+  </si>
+  <si>
+    <t>Pasteurella multocida (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus equi</t>
+  </si>
+  <si>
+    <t>Streptococcus equi (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus equi equi</t>
+  </si>
+  <si>
+    <t>Streptococcus equi subspecies equi (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus equi subspecies zooepidemicus (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus equi zooepidemicus</t>
+  </si>
+  <si>
+    <t>Streptococcus suis (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus suis</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1208,6 +1238,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1515,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1653,10 +1686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,573 +1822,628 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>224</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>241</v>
+        <v>380</v>
+      </c>
+      <c r="B12" s="5">
+        <v>10879005</v>
       </c>
       <c r="C12" t="s">
-        <v>240</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C13" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>236</v>
+        <v>337</v>
+      </c>
+      <c r="B15" t="s">
+        <v>304</v>
       </c>
       <c r="C15" t="s">
-        <v>237</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>229</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>238</v>
+        <v>327</v>
+      </c>
+      <c r="B16" t="s">
+        <v>269</v>
       </c>
       <c r="C16" t="s">
-        <v>239</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>218</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>219</v>
+        <v>336</v>
+      </c>
+      <c r="B17" t="s">
+        <v>303</v>
       </c>
       <c r="C17" t="s">
-        <v>220</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="B18" t="s">
-        <v>304</v>
+        <v>265</v>
       </c>
       <c r="C18" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="B20" t="s">
-        <v>303</v>
+        <v>266</v>
       </c>
       <c r="C20" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="B21" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C21" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B22" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="C22" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B23" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C23" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B24" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C24" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B25" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="B26" t="s">
-        <v>257</v>
+        <v>302</v>
       </c>
       <c r="C26" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B27" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C27" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B28" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C28" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="B29" t="s">
-        <v>302</v>
+        <v>260</v>
       </c>
       <c r="C29" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="B30" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="C30" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="B31" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="C31" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B32" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="C32" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B33" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C33" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B34" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C34" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B35" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C35" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="B36" t="s">
-        <v>270</v>
+        <v>305</v>
       </c>
       <c r="C36" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="B37" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="C37" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="B38" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C38" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B39" t="s">
-        <v>305</v>
+        <v>258</v>
       </c>
       <c r="C39" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B41" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C41" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B42" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C42" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="B43" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C43" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="B44" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C44" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>314</v>
-      </c>
-      <c r="B45" t="s">
-        <v>256</v>
+        <v>377</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="C45" t="s">
-        <v>281</v>
+        <v>375</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>329</v>
-      </c>
-      <c r="B46" t="s">
-        <v>271</v>
+        <v>226</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="C46" t="s">
-        <v>296</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>310</v>
-      </c>
-      <c r="B47" t="s">
-        <v>252</v>
+        <v>227</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="C47" t="s">
-        <v>277</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>377</v>
+        <v>228</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>376</v>
+        <v>236</v>
       </c>
       <c r="C48" t="s">
-        <v>375</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>49</v>
+      <c r="A49" t="s">
+        <v>229</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>50</v>
+        <v>238</v>
       </c>
       <c r="C49" t="s">
-        <v>51</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>244</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>246</v>
+        <v>382</v>
+      </c>
+      <c r="B50" s="5">
+        <v>12447002</v>
       </c>
       <c r="C50" t="s">
-        <v>245</v>
+        <v>383</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>248</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>249</v>
+        <v>384</v>
+      </c>
+      <c r="B51" s="5">
+        <v>113984001</v>
       </c>
       <c r="C51" t="s">
-        <v>250</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>339</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>365</v>
+        <v>387</v>
+      </c>
+      <c r="B52" s="5">
+        <v>33708000</v>
       </c>
       <c r="C52" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>340</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>353</v>
+        <v>389</v>
+      </c>
+      <c r="B53" s="5">
+        <v>7912006</v>
       </c>
       <c r="C53" t="s">
-        <v>354</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>355</v>
+      <c r="A54" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>357</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>356</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>358</v>
+        <v>244</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>359</v>
+        <v>246</v>
       </c>
       <c r="C55" t="s">
-        <v>360</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>341</v>
+        <v>248</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>350</v>
+        <v>249</v>
       </c>
       <c r="C56" t="s">
-        <v>349</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C57" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="C58" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="C59" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C60" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="C61" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="C62" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>343</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C63" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>344</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C64" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>345</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C65" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>346</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C66" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>347</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C67" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>348</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C68" t="s">
         <v>374</v>
       </c>
     </row>
@@ -2567,7 +2655,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Fixed General Diagnostic Code
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Mode</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>LabPIN</t>
   </si>
   <si>
@@ -1187,6 +1184,9 @@
   </si>
   <si>
     <t>Streptococcus suis</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1563,7 +1563,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,60 +1619,60 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
         <v>62</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" t="s">
         <v>242</v>
-      </c>
-      <c r="B14" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B15" s="2">
         <v>15</v>
@@ -1688,7 +1688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -1701,750 +1701,750 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C10" t="s">
         <v>221</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C10" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C11" t="s">
         <v>230</v>
-      </c>
-      <c r="C11" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B12" s="5">
         <v>10879005</v>
       </c>
       <c r="C12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" t="s">
         <v>219</v>
-      </c>
-      <c r="C14" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B28" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C38" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C43" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B44" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C44" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C45" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C46" t="s">
         <v>232</v>
-      </c>
-      <c r="C46" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C47" t="s">
         <v>234</v>
-      </c>
-      <c r="C47" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" t="s">
         <v>236</v>
-      </c>
-      <c r="C48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C49" t="s">
         <v>238</v>
-      </c>
-      <c r="C49" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B50" s="5">
         <v>12447002</v>
       </c>
       <c r="C50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B51" s="5">
         <v>113984001</v>
       </c>
       <c r="C51" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B52" s="5">
         <v>33708000</v>
       </c>
       <c r="C52" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B53" s="5">
         <v>7912006</v>
       </c>
       <c r="C53" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" t="s">
         <v>50</v>
-      </c>
-      <c r="C54" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>243</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" t="s">
         <v>244</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C55" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>247</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" t="s">
         <v>249</v>
-      </c>
-      <c r="C56" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C57" t="s">
         <v>365</v>
-      </c>
-      <c r="C57" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C58" t="s">
         <v>353</v>
-      </c>
-      <c r="C58" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>354</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C59" t="s">
         <v>355</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C59" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>357</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" t="s">
         <v>359</v>
-      </c>
-      <c r="C60" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C61" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C62" t="s">
         <v>361</v>
-      </c>
-      <c r="C62" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C63" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C64" t="s">
         <v>351</v>
-      </c>
-      <c r="C64" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C65" t="s">
         <v>367</v>
-      </c>
-      <c r="C65" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C66" t="s">
         <v>369</v>
-      </c>
-      <c r="C66" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C67" t="s">
         <v>371</v>
-      </c>
-      <c r="C67" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C68" t="s">
         <v>373</v>
-      </c>
-      <c r="C68" t="s">
-        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -2470,607 +2470,607 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" t="s">
         <v>215</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>216</v>
-      </c>
-      <c r="C4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C15" t="s">
         <v>211</v>
-      </c>
-      <c r="C15" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
+        <v>188</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B47" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B48" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
+        <v>196</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
+        <v>200</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B52" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
+        <v>204</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3084,7 +3084,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,57 +3096,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>389</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>389</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rebuild jar.  Additional mappings in config.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="461">
   <si>
     <t>Property</t>
   </si>
@@ -1187,6 +1187,219 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Idikan</t>
+  </si>
+  <si>
+    <t>Salmonella Idikan (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Litchfield</t>
+  </si>
+  <si>
+    <t>Salmonella Litchfield (organism)</t>
+  </si>
+  <si>
+    <t>Staphylococcus pseudImedius</t>
+  </si>
+  <si>
+    <t>Salmonella Stanley (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Stanley</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Give</t>
+  </si>
+  <si>
+    <t>Salmonella Give (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Ruiru</t>
+  </si>
+  <si>
+    <t>Salmonella Ruiru (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica rough 0:l,z13:1,5</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subspecies enterica serovar O rough: nonmotile (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica rough</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Rough</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Rough O:l,z13:1,5</t>
+  </si>
+  <si>
+    <t>Salmonella enterica O group B, HI, monophasic, unable to serotype further</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella enterica subspecies enterica serovar 4,5,12:i:- (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica Bovismorbificans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Bovismorbificans (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica 4,[5],12:i:-</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Mbdandaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Mbandaka (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica Sandiego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Sandiego (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella  enterica</t>
+  </si>
+  <si>
+    <t>Staphylococcus intermedius Group</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Kiambu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Kiambu (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica Oranienburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Oranienburg (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica 4, [5], 12:i:-</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Abony</t>
+  </si>
+  <si>
+    <t>Salmonella Abony (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica 4,[5], 12:i:-</t>
+  </si>
+  <si>
+    <t>Staph pseudintermedius</t>
+  </si>
+  <si>
+    <t>Salmonella enterica III 44:z4,z32:-</t>
+  </si>
+  <si>
+    <t>Salmonella IIIa 44:z4,z32:- (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica, Rough O:l,z13:1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella enterica subspecies enterica serovar O rough: nonmotile (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica rough O:eh:1,5</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Ealing</t>
+  </si>
+  <si>
+    <t>Salmonella Ealing (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica III 53:z4,z24:-</t>
+  </si>
+  <si>
+    <t>Salmonella IIIa 53:z4,z24:- (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Reading</t>
+  </si>
+  <si>
+    <t>Salmonella Reading (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Saintpaul</t>
+  </si>
+  <si>
+    <t>Salmonella Saintpaul (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Rough O:e,h:e,n,z15</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Telelkebir</t>
+  </si>
+  <si>
+    <t>Salmonella Telelkebir (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Hartford</t>
+  </si>
+  <si>
+    <t>Salmonella Hartford (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Liverpool</t>
+  </si>
+  <si>
+    <t>Salmonella Liverpool (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Panama</t>
+  </si>
+  <si>
+    <t>Salmonella Panama (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Carrau</t>
+  </si>
+  <si>
+    <t>Salmonella Carrau (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Bredeney</t>
+  </si>
+  <si>
+    <t>Salmonella Bredeney (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Norwich</t>
+  </si>
+  <si>
+    <t>Salmonella Norwich (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica 4,5,12:i:-</t>
+  </si>
+  <si>
+    <t>Salmonella enterica typhimurium</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Taksony</t>
+  </si>
+  <si>
+    <t>Salmonella Taksony (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica taksony</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Altona</t>
+  </si>
+  <si>
+    <t>Salmonella Altona (organism)</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1242,6 +1455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1548,7 +1762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1686,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,742 +1926,1207 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>346</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>222</v>
+        <v>370</v>
       </c>
       <c r="C10" t="s">
-        <v>221</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>379</v>
-      </c>
-      <c r="B12" s="5">
-        <v>10879005</v>
+        <v>342</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="C12" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="C13" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>217</v>
+      <c r="A14" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>218</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>336</v>
-      </c>
-      <c r="B15" t="s">
-        <v>303</v>
+        <v>243</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="C15" t="s">
-        <v>307</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>326</v>
-      </c>
-      <c r="B16" t="s">
-        <v>268</v>
+        <v>344</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>366</v>
       </c>
       <c r="C16" t="s">
-        <v>293</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>335</v>
-      </c>
-      <c r="B17" t="s">
-        <v>302</v>
+        <v>338</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>364</v>
       </c>
       <c r="C17" t="s">
-        <v>306</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>322</v>
-      </c>
-      <c r="B18" t="s">
-        <v>264</v>
+        <v>345</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>368</v>
       </c>
       <c r="C18" t="s">
-        <v>289</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>324</v>
-      </c>
-      <c r="B19" t="s">
-        <v>266</v>
+        <v>343</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="C19" t="s">
-        <v>291</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>323</v>
-      </c>
-      <c r="B20" t="s">
-        <v>265</v>
+        <v>339</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>352</v>
       </c>
       <c r="C20" t="s">
-        <v>290</v>
+        <v>353</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>330</v>
-      </c>
-      <c r="B21" t="s">
-        <v>272</v>
+        <v>357</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>358</v>
       </c>
       <c r="C21" t="s">
-        <v>297</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>331</v>
-      </c>
-      <c r="B22" t="s">
-        <v>273</v>
+        <v>354</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>356</v>
       </c>
       <c r="C22" t="s">
-        <v>298</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>314</v>
-      </c>
-      <c r="B23" t="s">
-        <v>256</v>
+        <v>340</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="C23" t="s">
-        <v>281</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>321</v>
-      </c>
-      <c r="B24" t="s">
-        <v>263</v>
+        <v>341</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>360</v>
       </c>
       <c r="C24" t="s">
-        <v>288</v>
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>329</v>
-      </c>
-      <c r="B25" t="s">
-        <v>271</v>
+        <v>347</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>372</v>
       </c>
       <c r="C25" t="s">
-        <v>296</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>334</v>
-      </c>
-      <c r="B26" t="s">
-        <v>301</v>
+        <v>224</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="C26" t="s">
-        <v>305</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>310</v>
-      </c>
-      <c r="B27" t="s">
-        <v>252</v>
+        <v>379</v>
+      </c>
+      <c r="B27" s="5">
+        <v>10879005</v>
       </c>
       <c r="C27" t="s">
-        <v>277</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>333</v>
-      </c>
-      <c r="B28" t="s">
-        <v>275</v>
+        <v>415</v>
+      </c>
+      <c r="B28" s="6">
+        <v>398508004</v>
       </c>
       <c r="C28" t="s">
-        <v>300</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>317</v>
-      </c>
-      <c r="B29" t="s">
-        <v>259</v>
+        <v>223</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="C29" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
       <c r="B30" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="C30" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="B31" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C31" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="B32" t="s">
-        <v>269</v>
+        <v>304</v>
       </c>
       <c r="C32" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B33" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C33" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="B34" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="C34" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B35" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C35" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B36" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
       <c r="C36" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B37" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C37" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="B38" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C38" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B39" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C39" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="B40" t="s">
-        <v>260</v>
+        <v>301</v>
       </c>
       <c r="C40" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B41" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C41" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="B42" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="C42" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="B43" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="C43" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="B44" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="C44" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>376</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>375</v>
+        <v>322</v>
+      </c>
+      <c r="B45" t="s">
+        <v>264</v>
       </c>
       <c r="C45" t="s">
-        <v>374</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>225</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>231</v>
+        <v>336</v>
+      </c>
+      <c r="B46" t="s">
+        <v>303</v>
       </c>
       <c r="C46" t="s">
-        <v>232</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>226</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>233</v>
+        <v>324</v>
+      </c>
+      <c r="B47" t="s">
+        <v>266</v>
       </c>
       <c r="C47" t="s">
-        <v>234</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>227</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>235</v>
+        <v>332</v>
+      </c>
+      <c r="B48" t="s">
+        <v>274</v>
       </c>
       <c r="C48" t="s">
-        <v>236</v>
+        <v>299</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>228</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>237</v>
+        <v>315</v>
+      </c>
+      <c r="B49" t="s">
+        <v>257</v>
       </c>
       <c r="C49" t="s">
-        <v>238</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>381</v>
-      </c>
-      <c r="B50" s="5">
-        <v>12447002</v>
+        <v>325</v>
+      </c>
+      <c r="B50" t="s">
+        <v>267</v>
       </c>
       <c r="C50" t="s">
-        <v>382</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>383</v>
-      </c>
-      <c r="B51" s="5">
-        <v>113984001</v>
+        <v>327</v>
+      </c>
+      <c r="B51" t="s">
+        <v>269</v>
       </c>
       <c r="C51" t="s">
-        <v>384</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>386</v>
-      </c>
-      <c r="B52" s="5">
-        <v>33708000</v>
+        <v>317</v>
+      </c>
+      <c r="B52" t="s">
+        <v>259</v>
       </c>
       <c r="C52" t="s">
-        <v>385</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>388</v>
-      </c>
-      <c r="B53" s="5">
-        <v>7912006</v>
+        <v>333</v>
+      </c>
+      <c r="B53" t="s">
+        <v>275</v>
       </c>
       <c r="C53" t="s">
-        <v>387</v>
+        <v>300</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>49</v>
+      <c r="A54" t="s">
+        <v>323</v>
+      </c>
+      <c r="B54" t="s">
+        <v>265</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>290</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>243</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>245</v>
+        <v>335</v>
+      </c>
+      <c r="B55" t="s">
+        <v>302</v>
       </c>
       <c r="C55" t="s">
-        <v>244</v>
+        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>247</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>248</v>
+        <v>310</v>
+      </c>
+      <c r="B56" t="s">
+        <v>252</v>
       </c>
       <c r="C56" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>338</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>364</v>
+        <v>326</v>
+      </c>
+      <c r="B57" t="s">
+        <v>268</v>
       </c>
       <c r="C57" t="s">
-        <v>365</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>339</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>352</v>
+        <v>330</v>
+      </c>
+      <c r="B58" t="s">
+        <v>272</v>
       </c>
       <c r="C58" t="s">
-        <v>353</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>354</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>356</v>
+        <v>421</v>
+      </c>
+      <c r="B59" s="6">
+        <v>442455001</v>
       </c>
       <c r="C59" t="s">
-        <v>355</v>
+        <v>407</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>357</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>358</v>
+        <v>424</v>
+      </c>
+      <c r="B60" s="6">
+        <v>442455001</v>
       </c>
       <c r="C60" t="s">
-        <v>359</v>
+        <v>407</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>340</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>349</v>
+        <v>410</v>
+      </c>
+      <c r="B61" s="6">
+        <v>442455001</v>
       </c>
       <c r="C61" t="s">
-        <v>348</v>
+        <v>407</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>341</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>360</v>
+        <v>454</v>
+      </c>
+      <c r="B62" s="6">
+        <v>442455001</v>
       </c>
       <c r="C62" t="s">
-        <v>361</v>
+        <v>407</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>342</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>363</v>
+        <v>422</v>
+      </c>
+      <c r="B63" s="6">
+        <v>40369005</v>
       </c>
       <c r="C63" t="s">
-        <v>362</v>
+        <v>423</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>343</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>350</v>
+        <v>459</v>
+      </c>
+      <c r="B64" s="6">
+        <v>47229009</v>
       </c>
       <c r="C64" t="s">
-        <v>351</v>
+        <v>460</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>344</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>366</v>
+        <v>408</v>
+      </c>
+      <c r="B65" s="6">
+        <v>81938008</v>
       </c>
       <c r="C65" t="s">
-        <v>367</v>
+        <v>409</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>345</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>368</v>
+        <v>450</v>
+      </c>
+      <c r="B66" s="6">
+        <v>82364007</v>
       </c>
       <c r="C66" t="s">
-        <v>369</v>
+        <v>451</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>346</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>370</v>
+        <v>448</v>
+      </c>
+      <c r="B67" s="6">
+        <v>32624003</v>
       </c>
       <c r="C67" t="s">
-        <v>371</v>
+        <v>449</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>347</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>372</v>
+        <v>431</v>
+      </c>
+      <c r="B68" s="6">
+        <v>15319009</v>
       </c>
       <c r="C68" t="s">
-        <v>373</v>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>397</v>
+      </c>
+      <c r="B69" s="6">
+        <v>71768003</v>
+      </c>
+      <c r="C69" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>442</v>
+      </c>
+      <c r="B70" s="6">
+        <v>26463008</v>
+      </c>
+      <c r="C70" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>390</v>
+      </c>
+      <c r="B71" s="6">
+        <v>52400005</v>
+      </c>
+      <c r="C71" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>426</v>
+      </c>
+      <c r="B72" s="6">
+        <v>404476005</v>
+      </c>
+      <c r="C72" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>433</v>
+      </c>
+      <c r="B73" s="6">
+        <v>416641008</v>
+      </c>
+      <c r="C73" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>417</v>
+      </c>
+      <c r="B74" s="6">
+        <v>11901002</v>
+      </c>
+      <c r="C74" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>392</v>
+      </c>
+      <c r="B75" s="6">
+        <v>81614007</v>
+      </c>
+      <c r="C75" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>444</v>
+      </c>
+      <c r="B76" s="6">
+        <v>25767003</v>
+      </c>
+      <c r="C76" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>411</v>
+      </c>
+      <c r="B77" s="6">
+        <v>9506004</v>
+      </c>
+      <c r="C77" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>217</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C78" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>452</v>
+      </c>
+      <c r="B79" s="6">
+        <v>10556004</v>
+      </c>
+      <c r="C79" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>406</v>
+      </c>
+      <c r="B80" s="6">
+        <v>442455001</v>
+      </c>
+      <c r="C80" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>376</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C81" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>419</v>
+      </c>
+      <c r="B82" s="6">
+        <v>46667007</v>
+      </c>
+      <c r="C82" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>446</v>
+      </c>
+      <c r="B83" s="6">
+        <v>40114001</v>
+      </c>
+      <c r="C83" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>435</v>
+      </c>
+      <c r="B84" s="6">
+        <v>63396002</v>
+      </c>
+      <c r="C84" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>403</v>
+      </c>
+      <c r="B85" s="6">
+        <v>721062001</v>
+      </c>
+      <c r="C85" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>404</v>
+      </c>
+      <c r="B86" s="6">
+        <v>721062001</v>
+      </c>
+      <c r="C86" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>401</v>
+      </c>
+      <c r="B87" s="6">
+        <v>721062001</v>
+      </c>
+      <c r="C87" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>439</v>
+      </c>
+      <c r="B88" s="6">
+        <v>721062001</v>
+      </c>
+      <c r="C88" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>430</v>
+      </c>
+      <c r="B89" s="6">
+        <v>721062001</v>
+      </c>
+      <c r="C89" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>405</v>
+      </c>
+      <c r="B90" s="6">
+        <v>721062001</v>
+      </c>
+      <c r="C90" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>399</v>
+      </c>
+      <c r="B91" s="6">
+        <v>25520000</v>
+      </c>
+      <c r="C91" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>437</v>
+      </c>
+      <c r="B92" s="6">
+        <v>2820001</v>
+      </c>
+      <c r="C92" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>413</v>
+      </c>
+      <c r="B93" s="6">
+        <v>112287008</v>
+      </c>
+      <c r="C93" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>396</v>
+      </c>
+      <c r="B94" s="6">
+        <v>88091007</v>
+      </c>
+      <c r="C94" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>456</v>
+      </c>
+      <c r="B95" s="6">
+        <v>33296009</v>
+      </c>
+      <c r="C95" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>458</v>
+      </c>
+      <c r="B96" s="6">
+        <v>33296009</v>
+      </c>
+      <c r="C96" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>440</v>
+      </c>
+      <c r="B97" s="6">
+        <v>64636003</v>
+      </c>
+      <c r="C97" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>455</v>
+      </c>
+      <c r="B98" s="6">
+        <v>50136005</v>
+      </c>
+      <c r="C98" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>428</v>
+      </c>
+      <c r="B99" s="6">
+        <v>721062001</v>
+      </c>
+      <c r="C99" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>425</v>
+      </c>
+      <c r="B100" s="6">
+        <v>427316000</v>
+      </c>
+      <c r="C100" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>228</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C101" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>226</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C102" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>416</v>
+      </c>
+      <c r="B103" s="6">
+        <v>719237009</v>
+      </c>
+      <c r="C103" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>225</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C104" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>394</v>
+      </c>
+      <c r="B105" s="6">
+        <v>427316000</v>
+      </c>
+      <c r="C105" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>227</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C106" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>381</v>
+      </c>
+      <c r="B107" s="5">
+        <v>12447002</v>
+      </c>
+      <c r="C107" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>383</v>
+      </c>
+      <c r="B108" s="5">
+        <v>113984001</v>
+      </c>
+      <c r="C108" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>386</v>
+      </c>
+      <c r="B109" s="5">
+        <v>33708000</v>
+      </c>
+      <c r="C109" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>388</v>
+      </c>
+      <c r="B110" s="5">
+        <v>7912006</v>
+      </c>
+      <c r="C110" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C110">
+    <sortCondition ref="A2:A110"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update sample Config file.  Add some logging.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -736,9 +736,6 @@
     <t>ProfileID</t>
   </si>
   <si>
-    <t>NAHLNResultBase_1_0_9_5</t>
-  </si>
-  <si>
     <t>lung</t>
   </si>
   <si>
@@ -1144,262 +1141,265 @@
     <t>General diagnostic testing</t>
   </si>
   <si>
+    <t>Pasteurella multocida</t>
+  </si>
+  <si>
+    <t>Pasteurella multocida (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus equi</t>
+  </si>
+  <si>
+    <t>Streptococcus equi (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus equi equi</t>
+  </si>
+  <si>
+    <t>Streptococcus equi subspecies equi (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus equi subspecies zooepidemicus (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus equi zooepidemicus</t>
+  </si>
+  <si>
+    <t>Streptococcus suis (organism)</t>
+  </si>
+  <si>
+    <t>Streptococcus suis</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Idikan</t>
+  </si>
+  <si>
+    <t>Salmonella Idikan (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Litchfield</t>
+  </si>
+  <si>
+    <t>Salmonella Litchfield (organism)</t>
+  </si>
+  <si>
+    <t>Staphylococcus pseudImedius</t>
+  </si>
+  <si>
+    <t>Salmonella Stanley (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Stanley</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Give</t>
+  </si>
+  <si>
+    <t>Salmonella Give (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Ruiru</t>
+  </si>
+  <si>
+    <t>Salmonella Ruiru (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica rough 0:l,z13:1,5</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subspecies enterica serovar O rough: nonmotile (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica rough</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Rough</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Rough O:l,z13:1,5</t>
+  </si>
+  <si>
+    <t>Salmonella enterica O group B, HI, monophasic, unable to serotype further</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella enterica subspecies enterica serovar 4,5,12:i:- (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica Bovismorbificans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Bovismorbificans (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica 4,[5],12:i:-</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Mbdandaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Mbandaka (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica Sandiego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Sandiego (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella  enterica</t>
+  </si>
+  <si>
+    <t>Staphylococcus intermedius Group</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Kiambu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Kiambu (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica Oranienburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella Oranienburg (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica 4, [5], 12:i:-</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Abony</t>
+  </si>
+  <si>
+    <t>Salmonella Abony (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica 4,[5], 12:i:-</t>
+  </si>
+  <si>
+    <t>Staph pseudintermedius</t>
+  </si>
+  <si>
+    <t>Salmonella enterica III 44:z4,z32:-</t>
+  </si>
+  <si>
+    <t>Salmonella IIIa 44:z4,z32:- (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica, Rough O:l,z13:1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella enterica subspecies enterica serovar O rough: nonmotile (organism) </t>
+  </si>
+  <si>
+    <t>Salmonella enterica rough O:eh:1,5</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Ealing</t>
+  </si>
+  <si>
+    <t>Salmonella Ealing (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica III 53:z4,z24:-</t>
+  </si>
+  <si>
+    <t>Salmonella IIIa 53:z4,z24:- (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Reading</t>
+  </si>
+  <si>
+    <t>Salmonella Reading (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Saintpaul</t>
+  </si>
+  <si>
+    <t>Salmonella Saintpaul (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Rough O:e,h:e,n,z15</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Telelkebir</t>
+  </si>
+  <si>
+    <t>Salmonella Telelkebir (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Hartford</t>
+  </si>
+  <si>
+    <t>Salmonella Hartford (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Liverpool</t>
+  </si>
+  <si>
+    <t>Salmonella Liverpool (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Panama</t>
+  </si>
+  <si>
+    <t>Salmonella Panama (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Carrau</t>
+  </si>
+  <si>
+    <t>Salmonella Carrau (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Bredeney</t>
+  </si>
+  <si>
+    <t>Salmonella Bredeney (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Norwich</t>
+  </si>
+  <si>
+    <t>Salmonella Norwich (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica 4,5,12:i:-</t>
+  </si>
+  <si>
+    <t>Salmonella enterica typhimurium</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Taksony</t>
+  </si>
+  <si>
+    <t>Salmonella Taksony (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica taksony</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Altona</t>
+  </si>
+  <si>
+    <t>Salmonella Altona (organism)</t>
+  </si>
+  <si>
+    <t>https://vsapps.aphis.usda.gov/HL7ResultTest</t>
+  </si>
+  <si>
+    <t>634-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bacteria identified in Unspecified specimen by Aerobe culture</t>
+  </si>
+  <si>
     <t>T</t>
   </si>
   <si>
-    <t>Pasteurella multocida</t>
-  </si>
-  <si>
-    <t>Pasteurella multocida (organism)</t>
-  </si>
-  <si>
-    <t>Streptococcus equi</t>
-  </si>
-  <si>
-    <t>Streptococcus equi (organism)</t>
-  </si>
-  <si>
-    <t>Streptococcus equi equi</t>
-  </si>
-  <si>
-    <t>Streptococcus equi subspecies equi (organism)</t>
-  </si>
-  <si>
-    <t>Streptococcus equi subspecies zooepidemicus (organism)</t>
-  </si>
-  <si>
-    <t>Streptococcus equi zooepidemicus</t>
-  </si>
-  <si>
-    <t>Streptococcus suis (organism)</t>
-  </si>
-  <si>
-    <t>Streptococcus suis</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Idikan</t>
-  </si>
-  <si>
-    <t>Salmonella Idikan (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Litchfield</t>
-  </si>
-  <si>
-    <t>Salmonella Litchfield (organism)</t>
-  </si>
-  <si>
-    <t>Staphylococcus pseudImedius</t>
-  </si>
-  <si>
-    <t>Salmonella Stanley (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Stanley</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Give</t>
-  </si>
-  <si>
-    <t>Salmonella Give (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Ruiru</t>
-  </si>
-  <si>
-    <t>Salmonella Ruiru (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica rough 0:l,z13:1,5</t>
-  </si>
-  <si>
-    <t>Salmonella enterica subspecies enterica serovar O rough: nonmotile (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica rough</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Rough</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Rough O:l,z13:1,5</t>
-  </si>
-  <si>
-    <t>Salmonella enterica O group B, HI, monophasic, unable to serotype further</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonella enterica subspecies enterica serovar 4,5,12:i:- (organism) </t>
-  </si>
-  <si>
-    <t>Salmonella enterica Bovismorbificans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonella Bovismorbificans (organism) </t>
-  </si>
-  <si>
-    <t>Salmonella enterica 4,[5],12:i:-</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Mbdandaka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonella Mbandaka (organism) </t>
-  </si>
-  <si>
-    <t>Salmonella enterica Sandiego</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonella Sandiego (organism) </t>
-  </si>
-  <si>
-    <t>Salmonella  enterica</t>
-  </si>
-  <si>
-    <t>Staphylococcus intermedius Group</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Kiambu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonella Kiambu (organism) </t>
-  </si>
-  <si>
-    <t>Salmonella enterica Oranienburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonella Oranienburg (organism) </t>
-  </si>
-  <si>
-    <t>Salmonella enterica 4, [5], 12:i:-</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Abony</t>
-  </si>
-  <si>
-    <t>Salmonella Abony (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica 4,[5], 12:i:-</t>
-  </si>
-  <si>
-    <t>Staph pseudintermedius</t>
-  </si>
-  <si>
-    <t>Salmonella enterica III 44:z4,z32:-</t>
-  </si>
-  <si>
-    <t>Salmonella IIIa 44:z4,z32:- (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica, Rough O:l,z13:1,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonella enterica subspecies enterica serovar O rough: nonmotile (organism) </t>
-  </si>
-  <si>
-    <t>Salmonella enterica rough O:eh:1,5</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Ealing</t>
-  </si>
-  <si>
-    <t>Salmonella Ealing (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica III 53:z4,z24:-</t>
-  </si>
-  <si>
-    <t>Salmonella IIIa 53:z4,z24:- (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Reading</t>
-  </si>
-  <si>
-    <t>Salmonella Reading (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Saintpaul</t>
-  </si>
-  <si>
-    <t>Salmonella Saintpaul (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Rough O:e,h:e,n,z15</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Telelkebir</t>
-  </si>
-  <si>
-    <t>Salmonella Telelkebir (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Hartford</t>
-  </si>
-  <si>
-    <t>Salmonella Hartford (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Liverpool</t>
-  </si>
-  <si>
-    <t>Salmonella Liverpool (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Panama</t>
-  </si>
-  <si>
-    <t>Salmonella Panama (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Carrau</t>
-  </si>
-  <si>
-    <t>Salmonella Carrau (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Bredeney</t>
-  </si>
-  <si>
-    <t>Salmonella Bredeney (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Norwich</t>
-  </si>
-  <si>
-    <t>Salmonella Norwich (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica 4,5,12:i:-</t>
-  </si>
-  <si>
-    <t>Salmonella enterica typhimurium</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Taksony</t>
-  </si>
-  <si>
-    <t>Salmonella Taksony (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica taksony</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Altona</t>
-  </si>
-  <si>
-    <t>Salmonella Altona (organism)</t>
-  </si>
-  <si>
-    <t>https://vsapps.aphis.usda.gov/HL7ResultTest</t>
-  </si>
-  <si>
-    <t>634-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bacteria identified in Unspecified specimen by Aerobe culture</t>
+    <t>NAHLNResultBaseV2.0</t>
   </si>
 </sst>
 </file>
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1844,7 +1844,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>375</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1884,7 +1884,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1892,12 +1892,12 @@
         <v>238</v>
       </c>
       <c r="B14" t="s">
-        <v>239</v>
+        <v>460</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B15" s="2">
         <v>15</v>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,35 +2028,35 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C10" t="s">
         <v>367</v>
-      </c>
-      <c r="C10" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" t="s">
         <v>245</v>
-      </c>
-      <c r="C11" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2083,123 +2083,123 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" t="s">
         <v>240</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C15" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C16" t="s">
         <v>363</v>
-      </c>
-      <c r="C16" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C17" t="s">
         <v>361</v>
-      </c>
-      <c r="C17" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C18" t="s">
         <v>365</v>
-      </c>
-      <c r="C18" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C19" t="s">
         <v>347</v>
-      </c>
-      <c r="C19" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C20" t="s">
         <v>349</v>
-      </c>
-      <c r="C20" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>353</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" t="s">
         <v>355</v>
-      </c>
-      <c r="C21" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>350</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C22" t="s">
         <v>351</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C22" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C24" t="s">
         <v>357</v>
-      </c>
-      <c r="C24" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C25" t="s">
         <v>369</v>
-      </c>
-      <c r="C25" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2215,18 +2215,18 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B27" s="5">
         <v>10879005</v>
       </c>
       <c r="C27" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B28" s="6">
         <v>398508004</v>
@@ -2248,530 +2248,530 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B35" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B41" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B42" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B43" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C43" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B44" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C45" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B46" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C46" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C50" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B51" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C51" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C52" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C53" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B54" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C54" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B55" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C55" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B56" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C56" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B57" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C57" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B58" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C58" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B59" s="6">
         <v>442455001</v>
       </c>
       <c r="C59" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B60" s="6">
         <v>442455001</v>
       </c>
       <c r="C60" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B61" s="6">
         <v>442455001</v>
       </c>
       <c r="C61" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B62" s="6">
         <v>442455001</v>
       </c>
       <c r="C62" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B63" s="6">
         <v>40369005</v>
       </c>
       <c r="C63" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B64" s="6">
         <v>47229009</v>
       </c>
       <c r="C64" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B65" s="6">
         <v>81938008</v>
       </c>
       <c r="C65" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B66" s="6">
         <v>82364007</v>
       </c>
       <c r="C66" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B67" s="6">
         <v>32624003</v>
       </c>
       <c r="C67" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B68" s="6">
         <v>15319009</v>
       </c>
       <c r="C68" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B69" s="6">
         <v>71768003</v>
       </c>
       <c r="C69" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B70" s="6">
         <v>26463008</v>
       </c>
       <c r="C70" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B71" s="6">
         <v>52400005</v>
       </c>
       <c r="C71" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B72" s="6">
         <v>404476005</v>
       </c>
       <c r="C72" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B73" s="6">
         <v>416641008</v>
       </c>
       <c r="C73" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B74" s="6">
         <v>11901002</v>
       </c>
       <c r="C74" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B75" s="6">
         <v>81614007</v>
       </c>
       <c r="C75" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B76" s="6">
         <v>25767003</v>
       </c>
       <c r="C76" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B77" s="6">
         <v>9506004</v>
       </c>
       <c r="C77" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2787,238 +2787,238 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B79" s="6">
         <v>10556004</v>
       </c>
       <c r="C79" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B80" s="6">
         <v>442455001</v>
       </c>
       <c r="C80" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C81" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B82" s="6">
         <v>46667007</v>
       </c>
       <c r="C82" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B83" s="6">
         <v>40114001</v>
       </c>
       <c r="C83" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B84" s="6">
         <v>63396002</v>
       </c>
       <c r="C84" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B85" s="6">
         <v>721062001</v>
       </c>
       <c r="C85" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B86" s="6">
         <v>721062001</v>
       </c>
       <c r="C86" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B87" s="6">
         <v>721062001</v>
       </c>
       <c r="C87" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B88" s="6">
         <v>721062001</v>
       </c>
       <c r="C88" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B89" s="6">
         <v>721062001</v>
       </c>
       <c r="C89" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B90" s="6">
         <v>721062001</v>
       </c>
       <c r="C90" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B91" s="6">
         <v>25520000</v>
       </c>
       <c r="C91" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B92" s="6">
         <v>2820001</v>
       </c>
       <c r="C92" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B93" s="6">
         <v>112287008</v>
       </c>
       <c r="C93" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B94" s="6">
         <v>88091007</v>
       </c>
       <c r="C94" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B95" s="6">
         <v>33296009</v>
       </c>
       <c r="C95" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B96" s="6">
         <v>33296009</v>
       </c>
       <c r="C96" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B97" s="6">
         <v>64636003</v>
       </c>
       <c r="C97" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B98" s="6">
         <v>50136005</v>
       </c>
       <c r="C98" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B99" s="6">
         <v>721062001</v>
       </c>
       <c r="C99" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B100" s="6">
         <v>427316000</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B103" s="6">
         <v>719237009</v>
@@ -3073,7 +3073,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B105" s="6">
         <v>427316000</v>
@@ -3095,46 +3095,46 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B107" s="5">
         <v>12447002</v>
       </c>
       <c r="C107" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B108" s="5">
         <v>113984001</v>
       </c>
       <c r="C108" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B109" s="5">
         <v>33708000</v>
       </c>
       <c r="C109" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B110" s="5">
         <v>7912006</v>
       </c>
       <c r="C110" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3150,7 +3150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -3199,10 +3199,10 @@
         <v>213</v>
       </c>
       <c r="B4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3803,7 +3803,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -3833,10 +3833,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Removed double spaces in Salmonella serotypes.  Added one serotype var.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="462">
   <si>
     <t>Property</t>
   </si>
@@ -934,93 +934,6 @@
     <t>Salmonella Albany (organism)</t>
   </si>
   <si>
-    <t>Salmonella enterica  4,[5],12:i:-</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Typhimurium</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Dublin</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Cerro</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Javiana</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Derby</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Montevideo</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Heidelberg</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Newport</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Agona</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Enteritidis</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Infantis</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Anatum</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Kentucky</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Senftenberg</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Mbandaka</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Muenchen</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Uganda</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Muenster</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Choleraesuis_(Kunzendorf)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Johannesburg</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Worthington</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Braenderup</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Meleagridis</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Rissen</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Hadar</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Thompson</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  London</t>
-  </si>
-  <si>
-    <t>Salmonella enterica  Albany</t>
-  </si>
-  <si>
     <t>Pharyngeal Swab</t>
   </si>
   <si>
@@ -1400,6 +1313,96 @@
   </si>
   <si>
     <t>NAHLNResultBaseV2.0</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Anatum var 15+</t>
+  </si>
+  <si>
+    <t>Salmonella Anatum var 15+ (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Agona</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Braenderup</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Cerro</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Choleraesuis_(Kunzendorf)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Derby</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Enteritidis</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Hadar</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Heidelberg</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Infantis</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Javiana</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Johannesburg</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Kentucky</t>
+  </si>
+  <si>
+    <t>Salmonella enterica London</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Mbandaka</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Meleagridis</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Montevideo</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Muenchen</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Muenster</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Newport</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Rissen</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Senftenberg</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Thompson</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Typhimurium</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Uganda</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Worthington</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Dublin</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Albany</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Anatum</t>
   </si>
 </sst>
 </file>
@@ -1457,15 +1460,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1773,7 +1776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1819,8 +1822,8 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>456</v>
+      <c r="B5" s="4" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1844,7 +1847,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>459</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1892,7 +1895,7 @@
         <v>238</v>
       </c>
       <c r="B14" t="s">
-        <v>460</v>
+        <v>431</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1914,16 +1917,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="68.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1931,7 +1934,7 @@
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C1" t="s">
@@ -1942,7 +1945,7 @@
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
@@ -1953,7 +1956,7 @@
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C3" t="s">
@@ -1964,7 +1967,7 @@
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C4" t="s">
@@ -1975,7 +1978,7 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C5" t="s">
@@ -1986,7 +1989,7 @@
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C6" t="s">
@@ -1997,7 +2000,7 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C7" t="s">
@@ -2008,7 +2011,7 @@
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
@@ -2019,7 +2022,7 @@
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C9" t="s">
@@ -2028,20 +2031,20 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>342</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>366</v>
+        <v>313</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>337</v>
       </c>
       <c r="C10" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>244</v>
       </c>
       <c r="C11" t="s">
@@ -2050,20 +2053,20 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>338</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>359</v>
+        <v>309</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>330</v>
       </c>
       <c r="C12" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>219</v>
       </c>
       <c r="C13" t="s">
@@ -2074,7 +2077,7 @@
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C14" t="s">
@@ -2085,7 +2088,7 @@
       <c r="A15" t="s">
         <v>239</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>241</v>
       </c>
       <c r="C15" t="s">
@@ -2094,119 +2097,119 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>340</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>362</v>
+        <v>311</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>333</v>
       </c>
       <c r="C16" t="s">
-        <v>363</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>334</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>360</v>
+        <v>305</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="C17" t="s">
-        <v>361</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>341</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>364</v>
+        <v>312</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>335</v>
       </c>
       <c r="C18" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>339</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>346</v>
+        <v>310</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>317</v>
       </c>
       <c r="C19" t="s">
-        <v>347</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>335</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>348</v>
+        <v>306</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>319</v>
       </c>
       <c r="C20" t="s">
-        <v>349</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>353</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>354</v>
+        <v>324</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>325</v>
       </c>
       <c r="C21" t="s">
-        <v>355</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>350</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>352</v>
+        <v>321</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>323</v>
       </c>
       <c r="C22" t="s">
-        <v>351</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>336</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>345</v>
+        <v>307</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>316</v>
       </c>
       <c r="C23" t="s">
-        <v>344</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>337</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>356</v>
+        <v>308</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>327</v>
       </c>
       <c r="C24" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>343</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>368</v>
+        <v>314</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>339</v>
       </c>
       <c r="C25" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>221</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>226</v>
       </c>
       <c r="C26" t="s">
@@ -2215,20 +2218,20 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>374</v>
-      </c>
-      <c r="B27" s="5">
+        <v>345</v>
+      </c>
+      <c r="B27" s="7">
         <v>10879005</v>
       </c>
       <c r="C27" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>410</v>
-      </c>
-      <c r="B28" s="6">
+        <v>381</v>
+      </c>
+      <c r="B28" s="5">
         <v>398508004</v>
       </c>
       <c r="C28" t="s">
@@ -2239,7 +2242,7 @@
       <c r="A29" t="s">
         <v>220</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>237</v>
       </c>
       <c r="C29" t="s">
@@ -2248,9 +2251,9 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>305</v>
-      </c>
-      <c r="B30" t="s">
+        <v>376</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>247</v>
       </c>
       <c r="C30" t="s">
@@ -2259,9 +2262,9 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>314</v>
-      </c>
-      <c r="B31" t="s">
+        <v>434</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>256</v>
       </c>
       <c r="C31" t="s">
@@ -2270,9 +2273,9 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>333</v>
-      </c>
-      <c r="B32" t="s">
+        <v>460</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>300</v>
       </c>
       <c r="C32" t="s">
@@ -2281,9 +2284,9 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>317</v>
-      </c>
-      <c r="B33" t="s">
+        <v>461</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>259</v>
       </c>
       <c r="C33" t="s">
@@ -2292,780 +2295,780 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>327</v>
-      </c>
-      <c r="B34" t="s">
-        <v>269</v>
+        <v>432</v>
+      </c>
+      <c r="B34" s="6">
+        <v>114274001</v>
       </c>
       <c r="C34" t="s">
-        <v>294</v>
+        <v>433</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>308</v>
-      </c>
-      <c r="B35" t="s">
-        <v>250</v>
+        <v>435</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="C35" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>324</v>
-      </c>
-      <c r="B36" t="s">
-        <v>266</v>
+        <v>436</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="C36" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>310</v>
-      </c>
-      <c r="B37" t="s">
-        <v>252</v>
+        <v>437</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="C37" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>307</v>
-      </c>
-      <c r="B38" t="s">
-        <v>249</v>
+        <v>438</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>252</v>
       </c>
       <c r="C38" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>315</v>
-      </c>
-      <c r="B39" t="s">
-        <v>257</v>
+        <v>459</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>249</v>
       </c>
       <c r="C39" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>330</v>
-      </c>
-      <c r="B40" t="s">
-        <v>297</v>
+        <v>439</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>257</v>
       </c>
       <c r="C40" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>312</v>
-      </c>
-      <c r="B41" t="s">
-        <v>254</v>
+        <v>440</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="C41" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>316</v>
-      </c>
-      <c r="B42" t="s">
-        <v>258</v>
+        <v>441</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>254</v>
       </c>
       <c r="C42" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>309</v>
-      </c>
-      <c r="B43" t="s">
-        <v>251</v>
+        <v>442</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>258</v>
       </c>
       <c r="C43" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>325</v>
-      </c>
-      <c r="B44" t="s">
-        <v>267</v>
+        <v>443</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>251</v>
       </c>
       <c r="C44" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>318</v>
-      </c>
-      <c r="B45" t="s">
-        <v>260</v>
+        <v>444</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="C45" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>332</v>
-      </c>
-      <c r="B46" t="s">
-        <v>299</v>
+        <v>445</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>260</v>
       </c>
       <c r="C46" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>320</v>
-      </c>
-      <c r="B47" t="s">
-        <v>262</v>
+        <v>446</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="C47" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>328</v>
-      </c>
-      <c r="B48" t="s">
-        <v>270</v>
+        <v>447</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>262</v>
       </c>
       <c r="C48" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>311</v>
-      </c>
-      <c r="B49" t="s">
-        <v>253</v>
+        <v>448</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="C49" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>321</v>
-      </c>
-      <c r="B50" t="s">
-        <v>263</v>
+        <v>449</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="C50" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>323</v>
-      </c>
-      <c r="B51" t="s">
-        <v>265</v>
+        <v>450</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="C51" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>313</v>
-      </c>
-      <c r="B52" t="s">
-        <v>255</v>
+        <v>451</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="C52" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>329</v>
-      </c>
-      <c r="B53" t="s">
-        <v>271</v>
+        <v>452</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="C53" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>319</v>
-      </c>
-      <c r="B54" t="s">
-        <v>261</v>
+        <v>453</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>271</v>
       </c>
       <c r="C54" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>331</v>
-      </c>
-      <c r="B55" t="s">
-        <v>298</v>
+        <v>454</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>261</v>
       </c>
       <c r="C55" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>306</v>
-      </c>
-      <c r="B56" t="s">
-        <v>248</v>
+        <v>455</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="C56" t="s">
-        <v>273</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>322</v>
-      </c>
-      <c r="B57" t="s">
-        <v>264</v>
+        <v>456</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>248</v>
       </c>
       <c r="C57" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>326</v>
-      </c>
-      <c r="B58" t="s">
-        <v>268</v>
+        <v>457</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>264</v>
       </c>
       <c r="C58" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>416</v>
-      </c>
-      <c r="B59" s="6">
-        <v>442455001</v>
+        <v>458</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="C59" t="s">
-        <v>402</v>
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>419</v>
+        <v>387</v>
       </c>
       <c r="B60" s="6">
         <v>442455001</v>
       </c>
       <c r="C60" t="s">
-        <v>402</v>
+        <v>373</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="B61" s="6">
         <v>442455001</v>
       </c>
       <c r="C61" t="s">
-        <v>402</v>
+        <v>373</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>449</v>
+        <v>376</v>
       </c>
       <c r="B62" s="6">
         <v>442455001</v>
       </c>
       <c r="C62" t="s">
-        <v>402</v>
+        <v>373</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B63" s="6">
-        <v>40369005</v>
+        <v>442455001</v>
       </c>
       <c r="C63" t="s">
-        <v>418</v>
+        <v>373</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>454</v>
+        <v>388</v>
       </c>
       <c r="B64" s="6">
-        <v>47229009</v>
+        <v>40369005</v>
       </c>
       <c r="C64" t="s">
-        <v>455</v>
+        <v>389</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>403</v>
+        <v>425</v>
       </c>
       <c r="B65" s="6">
-        <v>81938008</v>
+        <v>47229009</v>
       </c>
       <c r="C65" t="s">
-        <v>404</v>
+        <v>426</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>445</v>
+        <v>374</v>
       </c>
       <c r="B66" s="6">
-        <v>82364007</v>
+        <v>81938008</v>
       </c>
       <c r="C66" t="s">
-        <v>446</v>
+        <v>375</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>443</v>
+        <v>416</v>
       </c>
       <c r="B67" s="6">
-        <v>32624003</v>
+        <v>82364007</v>
       </c>
       <c r="C67" t="s">
-        <v>444</v>
+        <v>417</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="B68" s="6">
-        <v>15319009</v>
+        <v>32624003</v>
       </c>
       <c r="C68" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B69" s="6">
-        <v>71768003</v>
+        <v>15319009</v>
       </c>
       <c r="C69" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>437</v>
+        <v>363</v>
       </c>
       <c r="B70" s="6">
-        <v>26463008</v>
+        <v>71768003</v>
       </c>
       <c r="C70" t="s">
-        <v>438</v>
+        <v>364</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
       <c r="B71" s="6">
-        <v>52400005</v>
+        <v>26463008</v>
       </c>
       <c r="C71" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>421</v>
+        <v>356</v>
       </c>
       <c r="B72" s="6">
-        <v>404476005</v>
+        <v>52400005</v>
       </c>
       <c r="C72" t="s">
-        <v>422</v>
+        <v>357</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>428</v>
+        <v>392</v>
       </c>
       <c r="B73" s="6">
-        <v>416641008</v>
+        <v>404476005</v>
       </c>
       <c r="C73" t="s">
-        <v>429</v>
+        <v>393</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="B74" s="6">
-        <v>11901002</v>
+        <v>416641008</v>
       </c>
       <c r="C74" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B75" s="6">
-        <v>81614007</v>
+        <v>11901002</v>
       </c>
       <c r="C75" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>439</v>
+        <v>358</v>
       </c>
       <c r="B76" s="6">
-        <v>25767003</v>
+        <v>81614007</v>
       </c>
       <c r="C76" t="s">
-        <v>440</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B77" s="6">
-        <v>9506004</v>
+        <v>25767003</v>
       </c>
       <c r="C77" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>214</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>215</v>
+        <v>377</v>
+      </c>
+      <c r="B78" s="6">
+        <v>9506004</v>
       </c>
       <c r="C78" t="s">
-        <v>216</v>
+        <v>378</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>447</v>
-      </c>
-      <c r="B79" s="6">
-        <v>10556004</v>
+        <v>214</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="C79" t="s">
-        <v>448</v>
+        <v>216</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="B80" s="6">
-        <v>442455001</v>
+        <v>10556004</v>
       </c>
       <c r="C80" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>372</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>371</v>
+      <c r="B81" s="6">
+        <v>442455001</v>
       </c>
       <c r="C81" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>414</v>
-      </c>
-      <c r="B82" s="6">
-        <v>46667007</v>
+        <v>343</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="C82" t="s">
-        <v>415</v>
+        <v>341</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>441</v>
+        <v>385</v>
       </c>
       <c r="B83" s="6">
-        <v>40114001</v>
+        <v>46667007</v>
       </c>
       <c r="C83" t="s">
-        <v>442</v>
+        <v>386</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="B84" s="6">
-        <v>63396002</v>
+        <v>40114001</v>
       </c>
       <c r="C84" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B85" s="6">
-        <v>721062001</v>
+        <v>63396002</v>
       </c>
       <c r="C85" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>399</v>
+        <v>369</v>
       </c>
       <c r="B86" s="6">
         <v>721062001</v>
       </c>
       <c r="C86" t="s">
-        <v>397</v>
+        <v>368</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>396</v>
+        <v>370</v>
       </c>
       <c r="B87" s="6">
         <v>721062001</v>
       </c>
       <c r="C87" t="s">
-        <v>397</v>
+        <v>368</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>434</v>
+        <v>367</v>
       </c>
       <c r="B88" s="6">
         <v>721062001</v>
       </c>
       <c r="C88" t="s">
-        <v>397</v>
+        <v>368</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
       <c r="B89" s="6">
         <v>721062001</v>
       </c>
       <c r="C89" t="s">
-        <v>397</v>
+        <v>368</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B90" s="6">
         <v>721062001</v>
       </c>
       <c r="C90" t="s">
-        <v>397</v>
+        <v>368</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="B91" s="6">
-        <v>25520000</v>
+        <v>721062001</v>
       </c>
       <c r="C91" t="s">
-        <v>395</v>
+        <v>368</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>432</v>
+        <v>365</v>
       </c>
       <c r="B92" s="6">
-        <v>2820001</v>
+        <v>25520000</v>
       </c>
       <c r="C92" t="s">
-        <v>433</v>
+        <v>366</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B93" s="6">
-        <v>112287008</v>
+        <v>2820001</v>
       </c>
       <c r="C93" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="B94" s="6">
-        <v>88091007</v>
+        <v>112287008</v>
       </c>
       <c r="C94" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>451</v>
+        <v>362</v>
       </c>
       <c r="B95" s="6">
-        <v>33296009</v>
+        <v>88091007</v>
       </c>
       <c r="C95" t="s">
-        <v>452</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>453</v>
+        <v>422</v>
       </c>
       <c r="B96" s="6">
         <v>33296009</v>
       </c>
       <c r="C96" t="s">
-        <v>452</v>
+        <v>423</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="B97" s="6">
-        <v>64636003</v>
+        <v>33296009</v>
       </c>
       <c r="C97" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>450</v>
+        <v>406</v>
       </c>
       <c r="B98" s="6">
-        <v>50136005</v>
+        <v>64636003</v>
       </c>
       <c r="C98" t="s">
-        <v>273</v>
+        <v>407</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B99" s="6">
-        <v>721062001</v>
+        <v>50136005</v>
       </c>
       <c r="C99" t="s">
-        <v>424</v>
+        <v>273</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="B100" s="6">
-        <v>427316000</v>
+        <v>721062001</v>
       </c>
       <c r="C100" t="s">
-        <v>233</v>
+        <v>395</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>225</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>234</v>
+        <v>391</v>
+      </c>
+      <c r="B101" s="6">
+        <v>427316000</v>
       </c>
       <c r="C101" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>223</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="C102" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>411</v>
-      </c>
-      <c r="B103" s="6">
-        <v>719237009</v>
+        <v>223</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="C103" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>222</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>228</v>
+        <v>382</v>
+      </c>
+      <c r="B104" s="6">
+        <v>719237009</v>
       </c>
       <c r="C104" t="s">
         <v>229</v>
@@ -3073,21 +3076,21 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>389</v>
-      </c>
-      <c r="B105" s="6">
-        <v>427316000</v>
+        <v>222</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="C105" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>224</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>232</v>
+        <v>360</v>
+      </c>
+      <c r="B106" s="6">
+        <v>427316000</v>
       </c>
       <c r="C106" t="s">
         <v>233</v>
@@ -3095,46 +3098,57 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>376</v>
-      </c>
-      <c r="B107" s="5">
-        <v>12447002</v>
+        <v>224</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="C107" t="s">
-        <v>377</v>
+        <v>233</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>378</v>
-      </c>
-      <c r="B108" s="5">
-        <v>113984001</v>
+        <v>347</v>
+      </c>
+      <c r="B108" s="7">
+        <v>12447002</v>
       </c>
       <c r="C108" t="s">
-        <v>379</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>381</v>
-      </c>
-      <c r="B109" s="5">
-        <v>33708000</v>
+        <v>349</v>
+      </c>
+      <c r="B109" s="7">
+        <v>113984001</v>
       </c>
       <c r="C109" t="s">
-        <v>380</v>
+        <v>350</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>383</v>
-      </c>
-      <c r="B110" s="5">
+        <v>352</v>
+      </c>
+      <c r="B110" s="7">
+        <v>33708000</v>
+      </c>
+      <c r="C110" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>354</v>
+      </c>
+      <c r="B111" s="7">
         <v>7912006</v>
       </c>
-      <c r="C110" t="s">
-        <v>382</v>
+      <c r="C111" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -3199,10 +3213,10 @@
         <v>213</v>
       </c>
       <c r="B4" t="s">
-        <v>457</v>
+        <v>428</v>
       </c>
       <c r="C4" t="s">
-        <v>458</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3212,18 +3226,18 @@
       <c r="B5" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3234,7 +3248,7 @@
       <c r="B7" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3245,7 +3259,7 @@
       <c r="B8" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3256,7 +3270,7 @@
       <c r="B9" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3267,7 +3281,7 @@
       <c r="B10" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3278,7 +3292,7 @@
       <c r="B11" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3289,7 +3303,7 @@
       <c r="B12" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3300,7 +3314,7 @@
       <c r="B13" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3311,7 +3325,7 @@
       <c r="B14" t="s">
         <v>129</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3333,7 +3347,7 @@
       <c r="B16" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3344,7 +3358,7 @@
       <c r="B17" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3355,7 +3369,7 @@
       <c r="B18" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3366,7 +3380,7 @@
       <c r="B19" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3377,7 +3391,7 @@
       <c r="B20" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3388,7 +3402,7 @@
       <c r="B21" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3399,7 +3413,7 @@
       <c r="B22" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3410,7 +3424,7 @@
       <c r="B23" t="s">
         <v>145</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3421,7 +3435,7 @@
       <c r="B24" t="s">
         <v>145</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3432,7 +3446,7 @@
       <c r="B25" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3443,7 +3457,7 @@
       <c r="B26" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3454,7 +3468,7 @@
       <c r="B27" t="s">
         <v>151</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3465,7 +3479,7 @@
       <c r="B28" t="s">
         <v>153</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3476,7 +3490,7 @@
       <c r="B29" t="s">
         <v>155</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3487,7 +3501,7 @@
       <c r="B30" t="s">
         <v>157</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3498,7 +3512,7 @@
       <c r="B31" t="s">
         <v>159</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3509,7 +3523,7 @@
       <c r="B32" t="s">
         <v>161</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3520,7 +3534,7 @@
       <c r="B33" t="s">
         <v>163</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3531,7 +3545,7 @@
       <c r="B34" t="s">
         <v>165</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3542,7 +3556,7 @@
       <c r="B35" t="s">
         <v>167</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3553,7 +3567,7 @@
       <c r="B36" t="s">
         <v>169</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3564,7 +3578,7 @@
       <c r="B37" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3575,7 +3589,7 @@
       <c r="B38" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3586,7 +3600,7 @@
       <c r="B39" t="s">
         <v>175</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3597,7 +3611,7 @@
       <c r="B40" t="s">
         <v>177</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3608,7 +3622,7 @@
       <c r="B41" t="s">
         <v>179</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3619,7 +3633,7 @@
       <c r="B42" t="s">
         <v>181</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3630,7 +3644,7 @@
       <c r="B43" t="s">
         <v>183</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3641,7 +3655,7 @@
       <c r="B44" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3652,7 +3666,7 @@
       <c r="B45" t="s">
         <v>187</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3663,7 +3677,7 @@
       <c r="B46" t="s">
         <v>189</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3674,7 +3688,7 @@
       <c r="B47" t="s">
         <v>191</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3685,7 +3699,7 @@
       <c r="B48" t="s">
         <v>193</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3696,7 +3710,7 @@
       <c r="B49" t="s">
         <v>195</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3707,7 +3721,7 @@
       <c r="B50" t="s">
         <v>197</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>198</v>
       </c>
     </row>
@@ -3718,7 +3732,7 @@
       <c r="B51" t="s">
         <v>199</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3729,7 +3743,7 @@
       <c r="B52" t="s">
         <v>201</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3740,7 +3754,7 @@
       <c r="B53" t="s">
         <v>203</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3751,7 +3765,7 @@
       <c r="B54" t="s">
         <v>205</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3762,7 +3776,7 @@
       <c r="B55" t="s">
         <v>207</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3803,7 +3817,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -3833,10 +3847,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
       <c r="B5" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Parse out primary MIC from combination antibiotics.  Mapping values added.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="475">
   <si>
     <t>Property</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Meleagris gallopavo (organism)</t>
   </si>
   <si>
-    <t>Duck (organism)</t>
-  </si>
-  <si>
     <t>Genus Equus (organism)</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>20657003</t>
   </si>
   <si>
-    <t>29791000009109</t>
-  </si>
-  <si>
     <t>388445009</t>
   </si>
   <si>
@@ -1403,6 +1397,51 @@
   </si>
   <si>
     <t>Salmonella enterica Anatum</t>
+  </si>
+  <si>
+    <t>125102002</t>
+  </si>
+  <si>
+    <t>Anas platyrhynchos (organism)</t>
+  </si>
+  <si>
+    <t>Surveillance, National</t>
+  </si>
+  <si>
+    <t>Surveillance, Outbreak</t>
+  </si>
+  <si>
+    <t>Health Monitoring</t>
+  </si>
+  <si>
+    <t>General Diagnostics</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>abscess fluid</t>
+  </si>
+  <si>
+    <t>119371008</t>
+  </si>
+  <si>
+    <t>Specimen from abscess (specimen)</t>
+  </si>
+  <si>
+    <t>Lung</t>
+  </si>
+  <si>
+    <t>uterine swab</t>
+  </si>
+  <si>
+    <t>Feces</t>
+  </si>
+  <si>
+    <t>urine</t>
+  </si>
+  <si>
+    <t>Ear Swab</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1847,7 +1886,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1876,10 +1915,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1887,20 +1926,20 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B15" s="2">
         <v>15</v>
@@ -1917,10 +1956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,10 +1985,10 @@
         <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1957,7 +1996,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -1968,10 +2007,10 @@
         <v>27</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1979,10 +2018,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,7 +2029,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -2001,10 +2040,10 @@
         <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>41</v>
+        <v>460</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2012,7 +2051,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
@@ -2023,329 +2062,329 @@
         <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>313</v>
+      <c r="A10" s="1" t="s">
+        <v>467</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>337</v>
+        <v>468</v>
       </c>
       <c r="C10" t="s">
-        <v>338</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>243</v>
+        <v>311</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>244</v>
+        <v>335</v>
       </c>
       <c r="C11" t="s">
-        <v>245</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>309</v>
+        <v>241</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>330</v>
+        <v>242</v>
       </c>
       <c r="C12" t="s">
-        <v>329</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>474</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>219</v>
+        <v>328</v>
       </c>
       <c r="C13" t="s">
-        <v>218</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>47</v>
+      <c r="A14" t="s">
+        <v>307</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>328</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>311</v>
+      <c r="A16" s="1" t="s">
+        <v>472</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>333</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>334</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>305</v>
+      <c r="A17" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>331</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>332</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>312</v>
+        <v>237</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>335</v>
+        <v>239</v>
       </c>
       <c r="C18" t="s">
-        <v>336</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>310</v>
+        <v>470</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>317</v>
+        <v>239</v>
       </c>
       <c r="C19" t="s">
-        <v>318</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="C20" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C21" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="C22" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C23" t="s">
         <v>316</v>
-      </c>
-      <c r="C23" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="C24" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="C25" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>221</v>
+        <v>319</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>226</v>
+        <v>321</v>
       </c>
       <c r="C26" t="s">
-        <v>227</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>345</v>
-      </c>
-      <c r="B27" s="7">
-        <v>10879005</v>
+        <v>305</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>314</v>
       </c>
       <c r="C27" t="s">
-        <v>346</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>381</v>
-      </c>
-      <c r="B28" s="5">
-        <v>398508004</v>
+        <v>473</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>325</v>
       </c>
       <c r="C28" t="s">
-        <v>236</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>220</v>
+        <v>306</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>237</v>
+        <v>325</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>376</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>247</v>
+        <v>471</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>337</v>
       </c>
       <c r="C30" t="s">
-        <v>272</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>434</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>256</v>
+        <v>312</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>337</v>
       </c>
       <c r="C31" t="s">
-        <v>281</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>460</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>300</v>
+        <v>219</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="C32" t="s">
-        <v>304</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>461</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>259</v>
+        <v>343</v>
+      </c>
+      <c r="B33" s="7">
+        <v>10879005</v>
       </c>
       <c r="C33" t="s">
-        <v>284</v>
+        <v>344</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>432</v>
-      </c>
-      <c r="B34" s="6">
-        <v>114274001</v>
+        <v>379</v>
+      </c>
+      <c r="B34" s="5">
+        <v>398508004</v>
       </c>
       <c r="C34" t="s">
-        <v>433</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>435</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>269</v>
+        <v>218</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="C35" t="s">
-        <v>294</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>436</v>
+        <v>374</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C36" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C37" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>252</v>
+        <v>298</v>
       </c>
       <c r="C38" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2353,527 +2392,527 @@
         <v>459</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C39" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>439</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>257</v>
+        <v>430</v>
+      </c>
+      <c r="B40" s="6">
+        <v>114274001</v>
       </c>
       <c r="C40" t="s">
-        <v>282</v>
+        <v>431</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>297</v>
+        <v>267</v>
       </c>
       <c r="C41" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C42" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C43" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="C45" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C46" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C47" t="s">
         <v>299</v>
-      </c>
-      <c r="C47" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C48" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C49" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C50" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C51" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C52" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>255</v>
+        <v>297</v>
       </c>
       <c r="C53" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C54" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="C55" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>298</v>
+        <v>251</v>
       </c>
       <c r="C56" t="s">
-        <v>302</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="C57" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C58" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C59" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>387</v>
-      </c>
-      <c r="B60" s="6">
-        <v>442455001</v>
+        <v>451</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="C60" t="s">
-        <v>373</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>390</v>
-      </c>
-      <c r="B61" s="6">
-        <v>442455001</v>
+        <v>452</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="C61" t="s">
-        <v>373</v>
+        <v>284</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>376</v>
-      </c>
-      <c r="B62" s="6">
-        <v>442455001</v>
+        <v>453</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>296</v>
       </c>
       <c r="C62" t="s">
-        <v>373</v>
+        <v>300</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>420</v>
-      </c>
-      <c r="B63" s="6">
-        <v>442455001</v>
+        <v>454</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="C63" t="s">
-        <v>373</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>388</v>
-      </c>
-      <c r="B64" s="6">
-        <v>40369005</v>
+        <v>455</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>262</v>
       </c>
       <c r="C64" t="s">
-        <v>389</v>
+        <v>287</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>425</v>
-      </c>
-      <c r="B65" s="6">
-        <v>47229009</v>
+        <v>456</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="C65" t="s">
-        <v>426</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="B66" s="6">
-        <v>81938008</v>
+        <v>442455001</v>
       </c>
       <c r="C66" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>416</v>
+        <v>388</v>
       </c>
       <c r="B67" s="6">
-        <v>82364007</v>
+        <v>442455001</v>
       </c>
       <c r="C67" t="s">
-        <v>417</v>
+        <v>371</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
       <c r="B68" s="6">
-        <v>32624003</v>
+        <v>442455001</v>
       </c>
       <c r="C68" t="s">
-        <v>415</v>
+        <v>371</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>397</v>
+        <v>418</v>
       </c>
       <c r="B69" s="6">
-        <v>15319009</v>
+        <v>442455001</v>
       </c>
       <c r="C69" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>363</v>
+        <v>386</v>
       </c>
       <c r="B70" s="6">
-        <v>71768003</v>
+        <v>40369005</v>
       </c>
       <c r="C70" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>408</v>
+        <v>423</v>
       </c>
       <c r="B71" s="6">
-        <v>26463008</v>
+        <v>47229009</v>
       </c>
       <c r="C71" t="s">
-        <v>409</v>
+        <v>424</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>356</v>
+        <v>372</v>
       </c>
       <c r="B72" s="6">
-        <v>52400005</v>
+        <v>81938008</v>
       </c>
       <c r="C72" t="s">
-        <v>357</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>392</v>
+        <v>414</v>
       </c>
       <c r="B73" s="6">
-        <v>404476005</v>
+        <v>82364007</v>
       </c>
       <c r="C73" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>399</v>
+        <v>412</v>
       </c>
       <c r="B74" s="6">
-        <v>416641008</v>
+        <v>32624003</v>
       </c>
       <c r="C74" t="s">
-        <v>400</v>
+        <v>413</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="B75" s="6">
-        <v>11901002</v>
+        <v>15319009</v>
       </c>
       <c r="C75" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B76" s="6">
-        <v>81614007</v>
+        <v>71768003</v>
       </c>
       <c r="C76" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B77" s="6">
-        <v>25767003</v>
+        <v>26463008</v>
       </c>
       <c r="C77" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
       <c r="B78" s="6">
-        <v>9506004</v>
+        <v>52400005</v>
       </c>
       <c r="C78" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>214</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>215</v>
+        <v>390</v>
+      </c>
+      <c r="B79" s="6">
+        <v>404476005</v>
       </c>
       <c r="C79" t="s">
-        <v>216</v>
+        <v>391</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="B80" s="6">
-        <v>10556004</v>
+        <v>416641008</v>
       </c>
       <c r="C80" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="B81" s="6">
-        <v>442455001</v>
+        <v>11901002</v>
       </c>
       <c r="C81" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>343</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>342</v>
+        <v>356</v>
+      </c>
+      <c r="B82" s="6">
+        <v>81614007</v>
       </c>
       <c r="C82" t="s">
-        <v>341</v>
+        <v>357</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
       <c r="B83" s="6">
-        <v>46667007</v>
+        <v>25767003</v>
       </c>
       <c r="C83" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>412</v>
+        <v>375</v>
       </c>
       <c r="B84" s="6">
-        <v>40114001</v>
+        <v>9506004</v>
       </c>
       <c r="C84" t="s">
-        <v>413</v>
+        <v>376</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>401</v>
-      </c>
-      <c r="B85" s="6">
-        <v>63396002</v>
+        <v>212</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="C85" t="s">
-        <v>402</v>
+        <v>214</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>369</v>
+        <v>416</v>
       </c>
       <c r="B86" s="6">
-        <v>721062001</v>
+        <v>10556004</v>
       </c>
       <c r="C86" t="s">
-        <v>368</v>
+        <v>417</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2881,62 +2920,62 @@
         <v>370</v>
       </c>
       <c r="B87" s="6">
-        <v>721062001</v>
+        <v>442455001</v>
       </c>
       <c r="C87" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>367</v>
-      </c>
-      <c r="B88" s="6">
-        <v>721062001</v>
+        <v>341</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>340</v>
       </c>
       <c r="C88" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>405</v>
+        <v>383</v>
       </c>
       <c r="B89" s="6">
-        <v>721062001</v>
+        <v>46667007</v>
       </c>
       <c r="C89" t="s">
-        <v>368</v>
+        <v>384</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="B90" s="6">
-        <v>721062001</v>
+        <v>40114001</v>
       </c>
       <c r="C90" t="s">
-        <v>368</v>
+        <v>411</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>371</v>
+        <v>399</v>
       </c>
       <c r="B91" s="6">
-        <v>721062001</v>
+        <v>63396002</v>
       </c>
       <c r="C91" t="s">
-        <v>368</v>
+        <v>400</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B92" s="6">
-        <v>25520000</v>
+        <v>721062001</v>
       </c>
       <c r="C92" t="s">
         <v>366</v>
@@ -2944,211 +2983,277 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>403</v>
+        <v>368</v>
       </c>
       <c r="B93" s="6">
-        <v>2820001</v>
+        <v>721062001</v>
       </c>
       <c r="C93" t="s">
-        <v>404</v>
+        <v>366</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="B94" s="6">
-        <v>112287008</v>
+        <v>721062001</v>
       </c>
       <c r="C94" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>362</v>
+        <v>403</v>
       </c>
       <c r="B95" s="6">
-        <v>88091007</v>
+        <v>721062001</v>
       </c>
       <c r="C95" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>422</v>
+        <v>394</v>
       </c>
       <c r="B96" s="6">
-        <v>33296009</v>
+        <v>721062001</v>
       </c>
       <c r="C96" t="s">
-        <v>423</v>
+        <v>366</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>424</v>
+        <v>369</v>
       </c>
       <c r="B97" s="6">
-        <v>33296009</v>
+        <v>721062001</v>
       </c>
       <c r="C97" t="s">
-        <v>423</v>
+        <v>366</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>406</v>
+        <v>363</v>
       </c>
       <c r="B98" s="6">
-        <v>64636003</v>
+        <v>25520000</v>
       </c>
       <c r="C98" t="s">
-        <v>407</v>
+        <v>364</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="B99" s="6">
-        <v>50136005</v>
+        <v>2820001</v>
       </c>
       <c r="C99" t="s">
-        <v>273</v>
+        <v>402</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="B100" s="6">
-        <v>721062001</v>
+        <v>112287008</v>
       </c>
       <c r="C100" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>391</v>
+        <v>360</v>
       </c>
       <c r="B101" s="6">
-        <v>427316000</v>
+        <v>88091007</v>
       </c>
       <c r="C101" t="s">
-        <v>233</v>
+        <v>359</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>225</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>234</v>
+        <v>420</v>
+      </c>
+      <c r="B102" s="6">
+        <v>33296009</v>
       </c>
       <c r="C102" t="s">
-        <v>235</v>
+        <v>421</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>223</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>230</v>
+        <v>422</v>
+      </c>
+      <c r="B103" s="6">
+        <v>33296009</v>
       </c>
       <c r="C103" t="s">
-        <v>231</v>
+        <v>421</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>382</v>
+        <v>404</v>
       </c>
       <c r="B104" s="6">
-        <v>719237009</v>
+        <v>64636003</v>
       </c>
       <c r="C104" t="s">
-        <v>229</v>
+        <v>405</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>222</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>228</v>
+        <v>419</v>
+      </c>
+      <c r="B105" s="6">
+        <v>50136005</v>
       </c>
       <c r="C105" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>360</v>
+        <v>392</v>
       </c>
       <c r="B106" s="6">
-        <v>427316000</v>
+        <v>721062001</v>
       </c>
       <c r="C106" t="s">
-        <v>233</v>
+        <v>393</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>224</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>232</v>
+        <v>389</v>
+      </c>
+      <c r="B107" s="6">
+        <v>427316000</v>
       </c>
       <c r="C107" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>347</v>
-      </c>
-      <c r="B108" s="7">
-        <v>12447002</v>
+        <v>223</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="C108" t="s">
-        <v>348</v>
+        <v>233</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>349</v>
-      </c>
-      <c r="B109" s="7">
-        <v>113984001</v>
+        <v>221</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="C109" t="s">
-        <v>350</v>
+        <v>229</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>352</v>
-      </c>
-      <c r="B110" s="7">
-        <v>33708000</v>
+        <v>380</v>
+      </c>
+      <c r="B110" s="6">
+        <v>719237009</v>
       </c>
       <c r="C110" t="s">
-        <v>351</v>
+        <v>227</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>354</v>
-      </c>
-      <c r="B111" s="7">
+        <v>220</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C111" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>358</v>
+      </c>
+      <c r="B112" s="6">
+        <v>427316000</v>
+      </c>
+      <c r="C112" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>222</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C113" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>345</v>
+      </c>
+      <c r="B114" s="7">
+        <v>12447002</v>
+      </c>
+      <c r="C114" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>347</v>
+      </c>
+      <c r="B115" s="7">
+        <v>113984001</v>
+      </c>
+      <c r="C115" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>350</v>
+      </c>
+      <c r="B116" s="7">
+        <v>33708000</v>
+      </c>
+      <c r="C116" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>352</v>
+      </c>
+      <c r="B117" s="7">
         <v>7912006</v>
       </c>
-      <c r="C111" t="s">
-        <v>353</v>
+      <c r="C117" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -3188,596 +3293,596 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3788,10 +3893,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3814,49 +3919,94 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>462</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>463</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>464</v>
+      </c>
+      <c r="B8" t="s">
+        <v>466</v>
+      </c>
+      <c r="C8" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>465</v>
+      </c>
+      <c r="B9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Jan 2019 Build for Year 2
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="471">
   <si>
     <t>Property</t>
   </si>
@@ -121,12 +121,6 @@
     <t>Genus Equus (organism)</t>
   </si>
   <si>
-    <t>Canis lupus subspecies familiaris (organism)</t>
-  </si>
-  <si>
-    <t>Felis catus (organism)</t>
-  </si>
-  <si>
     <t>34618005</t>
   </si>
   <si>
@@ -142,12 +136,6 @@
     <t>388445009</t>
   </si>
   <si>
-    <t>448771007</t>
-  </si>
-  <si>
-    <t>448169003</t>
-  </si>
-  <si>
     <t>29548-5</t>
   </si>
   <si>
@@ -697,27 +685,15 @@
     <t>Mannheimia haemolytica (organism)</t>
   </si>
   <si>
-    <t>719237009</t>
-  </si>
-  <si>
     <t>Staphylococcus intermedius group (organism)</t>
   </si>
   <si>
-    <t>34605002</t>
-  </si>
-  <si>
     <t>Staphylococcus intermedius (organism)</t>
   </si>
   <si>
-    <t>427316000</t>
-  </si>
-  <si>
     <t>Staphylococcus pseudintermedius (organism)</t>
   </si>
   <si>
-    <t>113964000</t>
-  </si>
-  <si>
     <t>Staphylococcus delphini (organism)</t>
   </si>
   <si>
@@ -1057,9 +1033,6 @@
     <t>Streptococcus equi</t>
   </si>
   <si>
-    <t>Streptococcus equi (organism)</t>
-  </si>
-  <si>
     <t>Streptococcus equi equi</t>
   </si>
   <si>
@@ -1069,9 +1042,6 @@
     <t>Streptococcus equi subspecies zooepidemicus (organism)</t>
   </si>
   <si>
-    <t>Streptococcus equi zooepidemicus</t>
-  </si>
-  <si>
     <t>Streptococcus suis (organism)</t>
   </si>
   <si>
@@ -1303,145 +1273,163 @@
     <t xml:space="preserve"> Bacteria identified in Unspecified specimen by Aerobe culture</t>
   </si>
   <si>
+    <t>NAHLNResultBaseV2.0</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Anatum var 15+</t>
+  </si>
+  <si>
+    <t>Salmonella Anatum var 15+ (organism)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Agona</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Braenderup</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Cerro</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Choleraesuis_(Kunzendorf)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Derby</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Enteritidis</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Hadar</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Heidelberg</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Infantis</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Javiana</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Johannesburg</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Kentucky</t>
+  </si>
+  <si>
+    <t>Salmonella enterica London</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Mbandaka</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Meleagridis</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Montevideo</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Muenchen</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Muenster</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Newport</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Rissen</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Senftenberg</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Thompson</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Typhimurium</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Uganda</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Worthington</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Dublin</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Albany</t>
+  </si>
+  <si>
+    <t>Salmonella enterica Anatum</t>
+  </si>
+  <si>
+    <t>125102002</t>
+  </si>
+  <si>
+    <t>Anas platyrhynchos (organism)</t>
+  </si>
+  <si>
+    <t>Surveillance, National</t>
+  </si>
+  <si>
+    <t>Surveillance, Outbreak</t>
+  </si>
+  <si>
+    <t>Health Monitoring</t>
+  </si>
+  <si>
+    <t>General Diagnostics</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>abscess fluid</t>
+  </si>
+  <si>
+    <t>119371008</t>
+  </si>
+  <si>
+    <t>Specimen from abscess (specimen)</t>
+  </si>
+  <si>
+    <t>Lung</t>
+  </si>
+  <si>
+    <t>uterine swab</t>
+  </si>
+  <si>
+    <t>Feces</t>
+  </si>
+  <si>
+    <t>urine</t>
+  </si>
+  <si>
+    <t>Ear Swab</t>
+  </si>
+  <si>
+    <t>388626009</t>
+  </si>
+  <si>
+    <t>Genus Felis (organism)</t>
+  </si>
+  <si>
+    <t>388490000</t>
+  </si>
+  <si>
+    <t>Genus Canis (organism)</t>
+  </si>
+  <si>
+    <t>721062001</t>
+  </si>
+  <si>
+    <t>Streptococcus zooepidemicus</t>
+  </si>
+  <si>
     <t>T</t>
-  </si>
-  <si>
-    <t>NAHLNResultBaseV2.0</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Anatum var 15+</t>
-  </si>
-  <si>
-    <t>Salmonella Anatum var 15+ (organism)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Agona</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Braenderup</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Cerro</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Choleraesuis_(Kunzendorf)</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Derby</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Enteritidis</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Hadar</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Heidelberg</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Infantis</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Javiana</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Johannesburg</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Kentucky</t>
-  </si>
-  <si>
-    <t>Salmonella enterica London</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Mbandaka</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Meleagridis</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Montevideo</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Muenchen</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Muenster</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Newport</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Rissen</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Senftenberg</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Thompson</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Typhimurium</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Uganda</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Worthington</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Dublin</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Albany</t>
-  </si>
-  <si>
-    <t>Salmonella enterica Anatum</t>
-  </si>
-  <si>
-    <t>125102002</t>
-  </si>
-  <si>
-    <t>Anas platyrhynchos (organism)</t>
-  </si>
-  <si>
-    <t>Surveillance, National</t>
-  </si>
-  <si>
-    <t>Surveillance, Outbreak</t>
-  </si>
-  <si>
-    <t>Health Monitoring</t>
-  </si>
-  <si>
-    <t>General Diagnostics</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>abscess fluid</t>
-  </si>
-  <si>
-    <t>119371008</t>
-  </si>
-  <si>
-    <t>Specimen from abscess (specimen)</t>
-  </si>
-  <si>
-    <t>Lung</t>
-  </si>
-  <si>
-    <t>uterine swab</t>
-  </si>
-  <si>
-    <t>Feces</t>
-  </si>
-  <si>
-    <t>urine</t>
-  </si>
-  <si>
-    <t>Ear Swab</t>
   </si>
 </sst>
 </file>
@@ -1815,7 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1862,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1886,7 +1874,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>428</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1915,10 +1903,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1926,20 +1914,20 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B15" s="2">
         <v>15</v>
@@ -1958,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,10 +1973,10 @@
         <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>464</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1996,7 +1984,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -2007,10 +1995,10 @@
         <v>27</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>466</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2018,7 +2006,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -2029,7 +2017,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -2040,10 +2028,10 @@
         <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="C7" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2051,7 +2039,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
@@ -2062,7 +2050,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -2070,1190 +2058,1190 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="C10" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="C11" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C12" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C13" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C14" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C19" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C20" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="C21" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C22" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C23" t="s">
         <v>308</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="C23" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C24" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C25" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C26" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>297</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C27" t="s">
         <v>305</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="C27" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C28" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C29" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C30" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C31" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C32" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B33" s="7">
         <v>10879005</v>
       </c>
       <c r="C33" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="B34" s="5">
         <v>398508004</v>
       </c>
       <c r="C34" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C35" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C36" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C37" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C38" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C39" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="B40" s="6">
         <v>114274001</v>
       </c>
       <c r="C40" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C41" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C42" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C43" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C44" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C45" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C46" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="C47" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C48" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C49" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C50" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C51" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C52" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C53" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C54" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C55" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C56" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C57" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C58" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C59" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C60" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C61" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C62" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C63" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C64" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C65" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B66" s="6">
         <v>442455001</v>
       </c>
       <c r="C66" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="B67" s="6">
         <v>442455001</v>
       </c>
       <c r="C67" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B68" s="6">
         <v>442455001</v>
       </c>
       <c r="C68" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="B69" s="6">
         <v>442455001</v>
       </c>
       <c r="C69" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B70" s="6">
         <v>40369005</v>
       </c>
       <c r="C70" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B71" s="6">
         <v>47229009</v>
       </c>
       <c r="C71" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="B72" s="6">
         <v>81938008</v>
       </c>
       <c r="C72" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="B73" s="6">
         <v>82364007</v>
       </c>
       <c r="C73" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="B74" s="6">
         <v>32624003</v>
       </c>
       <c r="C74" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="B75" s="6">
         <v>15319009</v>
       </c>
       <c r="C75" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B76" s="6">
         <v>71768003</v>
       </c>
       <c r="C76" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="B77" s="6">
         <v>26463008</v>
       </c>
       <c r="C77" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B78" s="6">
         <v>52400005</v>
       </c>
       <c r="C78" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B79" s="6">
         <v>404476005</v>
       </c>
       <c r="C79" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="B80" s="6">
         <v>416641008</v>
       </c>
       <c r="C80" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B81" s="6">
         <v>11901002</v>
       </c>
       <c r="C81" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B82" s="6">
         <v>81614007</v>
       </c>
       <c r="C82" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="B83" s="6">
         <v>25767003</v>
       </c>
       <c r="C83" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B84" s="6">
         <v>9506004</v>
       </c>
       <c r="C84" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C85" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="B86" s="6">
         <v>10556004</v>
       </c>
       <c r="C86" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B87" s="6">
         <v>442455001</v>
       </c>
       <c r="C87" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C88" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="B89" s="6">
         <v>46667007</v>
       </c>
       <c r="C89" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="B90" s="6">
         <v>40114001</v>
       </c>
       <c r="C90" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="B91" s="6">
         <v>63396002</v>
       </c>
       <c r="C91" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="B92" s="6">
         <v>721062001</v>
       </c>
       <c r="C92" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B93" s="6">
         <v>721062001</v>
       </c>
       <c r="C93" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B94" s="6">
         <v>721062001</v>
       </c>
       <c r="C94" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="B95" s="6">
         <v>721062001</v>
       </c>
       <c r="C95" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="B96" s="6">
         <v>721062001</v>
       </c>
       <c r="C96" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="B97" s="6">
         <v>721062001</v>
       </c>
       <c r="C97" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B98" s="6">
         <v>25520000</v>
       </c>
       <c r="C98" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="B99" s="6">
         <v>2820001</v>
       </c>
       <c r="C99" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B100" s="6">
         <v>112287008</v>
       </c>
       <c r="C100" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B101" s="6">
         <v>88091007</v>
       </c>
       <c r="C101" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="B102" s="6">
         <v>33296009</v>
       </c>
       <c r="C102" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="B103" s="6">
         <v>33296009</v>
       </c>
       <c r="C103" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="B104" s="6">
         <v>64636003</v>
       </c>
       <c r="C104" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="B105" s="6">
         <v>50136005</v>
       </c>
       <c r="C105" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>392</v>
-      </c>
-      <c r="B106" s="6">
-        <v>721062001</v>
+        <v>382</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>468</v>
       </c>
       <c r="C106" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B107" s="6">
         <v>427316000</v>
       </c>
       <c r="C107" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>223</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>232</v>
+        <v>219</v>
+      </c>
+      <c r="B108" s="5">
+        <v>113964000</v>
       </c>
       <c r="C108" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>221</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>228</v>
+        <v>217</v>
+      </c>
+      <c r="B109" s="5">
+        <v>34605002</v>
       </c>
       <c r="C109" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="B110" s="6">
         <v>719237009</v>
       </c>
       <c r="C110" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>220</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>226</v>
+        <v>216</v>
+      </c>
+      <c r="B111" s="5">
+        <v>719237009</v>
       </c>
       <c r="C111" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B112" s="6">
         <v>427316000</v>
       </c>
       <c r="C112" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>230</v>
+        <v>218</v>
+      </c>
+      <c r="B113" s="5">
+        <v>427316000</v>
       </c>
       <c r="C113" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="B114" s="7">
-        <v>12447002</v>
+        <v>113984001</v>
       </c>
       <c r="C114" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B115" s="7">
         <v>113984001</v>
       </c>
       <c r="C115" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>350</v>
+        <v>469</v>
       </c>
       <c r="B116" s="7">
         <v>33708000</v>
       </c>
       <c r="C116" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B117" s="7">
         <v>7912006</v>
       </c>
       <c r="C117" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -3262,6 +3250,9 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B106" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -3293,596 +3284,596 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="C4" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B55" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3919,90 +3910,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="B5" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B8" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="C8" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="B9" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed empty first cell bug.  At least patched.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E15D84A-7671-48E6-B97F-CF08E89AA2F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="20325" yWindow="675" windowWidth="15525" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -1429,13 +1430,13 @@
     <t>Streptococcus zooepidemicus</t>
   </si>
   <si>
-    <t>T</t>
+    <t>D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1590,6 +1591,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1625,6 +1643,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1800,7 +1835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1935,7 +1970,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1943,7 +1978,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView topLeftCell="A90" workbookViewId="0">
@@ -3245,7 +3280,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C110">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C110">
     <sortCondition ref="A2:A110"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3257,7 +3292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3883,7 +3918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>